<commit_message>
-started creating SaiBotData.csv to use naive bayes classifier for chatbot responses rather than a chatbot API due to poor performance.
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{753765A2-CA6B-43B6-BD36-F49C6EAB83CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F737780-EC7C-487E-BC8F-BE2955E9819B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>prompt</t>
   </si>
@@ -81,6 +81,54 @@
   </si>
   <si>
     <t>I'm glad to hear that!</t>
+  </si>
+  <si>
+    <t>I feel tired</t>
+  </si>
+  <si>
+    <t>I am tired</t>
+  </si>
+  <si>
+    <t>im kinda tired today</t>
+  </si>
+  <si>
+    <t>I didn’t get much sleep last night</t>
+  </si>
+  <si>
+    <t>I wasn’t able to sleep at all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm sorry to hear that. If you have can, I would set aside some time to relax at some point this week. </t>
+  </si>
+  <si>
+    <t>Im very stressed out right now</t>
+  </si>
+  <si>
+    <t>Im so stressed</t>
+  </si>
+  <si>
+    <t>I don’t have any time for myself</t>
+  </si>
+  <si>
+    <t>I don’t have time to work on my homework</t>
+  </si>
+  <si>
+    <t>I don’t have time to relax</t>
+  </si>
+  <si>
+    <t>I wish I had time to relax</t>
+  </si>
+  <si>
+    <t>I havent been able to rest or relax</t>
+  </si>
+  <si>
+    <t>I need to rest</t>
+  </si>
+  <si>
+    <t>I need to calm down</t>
+  </si>
+  <si>
+    <t>I'm sorry to hear that. I'm sure you have a lot going on right now. It can be hard to make time for yourself to unwind and relax, but it is crucial to a healthy balance in life. If you would like, I can help you destress with one of my coping activities. If you're interested, please press the coping activities button on the right side of the screen. I hope you can unwind and feel better soon.</t>
   </si>
 </sst>
 </file>
@@ -432,15 +480,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="94.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -539,6 +588,118 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
-updated saibotdata and updated breathing activity
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F737780-EC7C-487E-BC8F-BE2955E9819B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10602067-3C1B-4750-B919-D54084D614F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
   <si>
     <t>prompt</t>
   </si>
@@ -98,9 +98,6 @@
     <t>I wasn’t able to sleep at all</t>
   </si>
   <si>
-    <t xml:space="preserve">I'm sorry to hear that. If you have can, I would set aside some time to relax at some point this week. </t>
-  </si>
-  <si>
     <t>Im very stressed out right now</t>
   </si>
   <si>
@@ -129,6 +126,141 @@
   </si>
   <si>
     <t>I'm sorry to hear that. I'm sure you have a lot going on right now. It can be hard to make time for yourself to unwind and relax, but it is crucial to a healthy balance in life. If you would like, I can help you destress with one of my coping activities. If you're interested, please press the coping activities button on the right side of the screen. I hope you can unwind and feel better soon.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'm sorry to hear that. If you can, I would set aside some time to relax at some point this week. </t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>greeting</t>
+  </si>
+  <si>
+    <t>feeling good</t>
+  </si>
+  <si>
+    <t>feeling tired</t>
+  </si>
+  <si>
+    <t>feeling stressed</t>
+  </si>
+  <si>
+    <t>Thank you</t>
+  </si>
+  <si>
+    <t>gratitude/appreciation</t>
+  </si>
+  <si>
+    <t>No problem, I am always happy to help!</t>
+  </si>
+  <si>
+    <t>thanks</t>
+  </si>
+  <si>
+    <t>I really appreciate it</t>
+  </si>
+  <si>
+    <t>im grateful</t>
+  </si>
+  <si>
+    <t>im grateful for your help</t>
+  </si>
+  <si>
+    <t>thanks again</t>
+  </si>
+  <si>
+    <t>im sorry</t>
+  </si>
+  <si>
+    <t>apology</t>
+  </si>
+  <si>
+    <t>It's okay, I don't mind. I am here to help you in any way I can.</t>
+  </si>
+  <si>
+    <t>I am sorry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I didn’t mean to </t>
+  </si>
+  <si>
+    <t>sorry</t>
+  </si>
+  <si>
+    <t>I apologize</t>
+  </si>
+  <si>
+    <t>I want to apologize for my behavior</t>
+  </si>
+  <si>
+    <t>I want to apologize</t>
+  </si>
+  <si>
+    <t>I want to say im sorry</t>
+  </si>
+  <si>
+    <t>how to apologize</t>
+  </si>
+  <si>
+    <t>how to calm down</t>
+  </si>
+  <si>
+    <t>how to ground</t>
+  </si>
+  <si>
+    <t>how to cope</t>
+  </si>
+  <si>
+    <t>how to make friends</t>
+  </si>
+  <si>
+    <t>how to build confidence</t>
+  </si>
+  <si>
+    <t>how to be less nervous</t>
+  </si>
+  <si>
+    <t>how to cheer up</t>
+  </si>
+  <si>
+    <t>how to cheer someone else up</t>
+  </si>
+  <si>
+    <t>who is Sai</t>
+  </si>
+  <si>
+    <t>who made Sai</t>
+  </si>
+  <si>
+    <t>Why does Sai want to help</t>
+  </si>
+  <si>
+    <t>why does sai care</t>
+  </si>
+  <si>
+    <t>what is depression</t>
+  </si>
+  <si>
+    <t>what is anxiety</t>
+  </si>
+  <si>
+    <t>what is schizophrenia</t>
+  </si>
+  <si>
+    <t>what is ocd</t>
+  </si>
+  <si>
+    <t>what is adhd</t>
+  </si>
+  <si>
+    <t>what is add</t>
+  </si>
+  <si>
+    <t>what is an eating disorder</t>
+  </si>
+  <si>
+    <t>what is suicidal ideation</t>
   </si>
 </sst>
 </file>
@@ -480,224 +612,661 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="94.21875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="131.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>23</v>
       </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
-      <c r="B23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="B33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>27</v>
       </c>
-      <c r="B24" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>28</v>
       </c>
-      <c r="B25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="B35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C35" t="s">
         <v>29</v>
       </c>
-      <c r="B26" t="s">
-        <v>30</v>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>37</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>37</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-updated saibotdata.csv and .xlsx -added text_cleanup to chatbot classifier
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{10602067-3C1B-4750-B919-D54084D614F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA07A2CA-B1C7-4141-8F3F-BA4E2AF6DB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
@@ -200,67 +200,67 @@
     <t>I want to say im sorry</t>
   </si>
   <si>
+    <t>what is suicidal ideation</t>
+  </si>
+  <si>
+    <t>what is an eating disorder</t>
+  </si>
+  <si>
+    <t>what is add</t>
+  </si>
+  <si>
+    <t>what is adhd</t>
+  </si>
+  <si>
+    <t>what is ocd</t>
+  </si>
+  <si>
+    <t>what is schizophrenia</t>
+  </si>
+  <si>
+    <t>what is anxiety</t>
+  </si>
+  <si>
+    <t>what is depression</t>
+  </si>
+  <si>
+    <t>why does sai care</t>
+  </si>
+  <si>
+    <t>Why does Sai want to help</t>
+  </si>
+  <si>
+    <t>who made Sai</t>
+  </si>
+  <si>
+    <t>who is Sai</t>
+  </si>
+  <si>
+    <t>how to cheer someone else up</t>
+  </si>
+  <si>
+    <t>how to cheer up</t>
+  </si>
+  <si>
+    <t>how to be less nervous</t>
+  </si>
+  <si>
+    <t>how to build confidence</t>
+  </si>
+  <si>
+    <t>how to make friends</t>
+  </si>
+  <si>
+    <t>how to cope</t>
+  </si>
+  <si>
+    <t>how to ground</t>
+  </si>
+  <si>
+    <t>how to calm down</t>
+  </si>
+  <si>
     <t>how to apologize</t>
-  </si>
-  <si>
-    <t>how to calm down</t>
-  </si>
-  <si>
-    <t>how to ground</t>
-  </si>
-  <si>
-    <t>how to cope</t>
-  </si>
-  <si>
-    <t>how to make friends</t>
-  </si>
-  <si>
-    <t>how to build confidence</t>
-  </si>
-  <si>
-    <t>how to be less nervous</t>
-  </si>
-  <si>
-    <t>how to cheer up</t>
-  </si>
-  <si>
-    <t>how to cheer someone else up</t>
-  </si>
-  <si>
-    <t>who is Sai</t>
-  </si>
-  <si>
-    <t>who made Sai</t>
-  </si>
-  <si>
-    <t>Why does Sai want to help</t>
-  </si>
-  <si>
-    <t>why does sai care</t>
-  </si>
-  <si>
-    <t>what is depression</t>
-  </si>
-  <si>
-    <t>what is anxiety</t>
-  </si>
-  <si>
-    <t>what is schizophrenia</t>
-  </si>
-  <si>
-    <t>what is ocd</t>
-  </si>
-  <si>
-    <t>what is adhd</t>
-  </si>
-  <si>
-    <t>what is add</t>
-  </si>
-  <si>
-    <t>what is an eating disorder</t>
-  </si>
-  <si>
-    <t>what is suicidal ideation</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B50" sqref="B50:B70"/>
     </sheetView>
   </sheetViews>
@@ -1166,52 +1166,52 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1221,52 +1221,52 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-started working on results page.
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA07A2CA-B1C7-4141-8F3F-BA4E2AF6DB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BE3389A-8B42-4F1B-8618-FD7B125D90CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="212" uniqueCount="93">
   <si>
     <t>prompt</t>
   </si>
@@ -200,6 +203,90 @@
     <t>I want to say im sorry</t>
   </si>
   <si>
+    <t>Why does Sai want to help</t>
+  </si>
+  <si>
+    <t>who made Sai</t>
+  </si>
+  <si>
+    <t>who is Sai</t>
+  </si>
+  <si>
+    <t>who are you</t>
+  </si>
+  <si>
+    <t>what are you</t>
+  </si>
+  <si>
+    <t>tell me your name</t>
+  </si>
+  <si>
+    <t>what is your name</t>
+  </si>
+  <si>
+    <t>My name is Sai. I am an Emotional Support AI designed to help people talk about and handle their emotions.</t>
+  </si>
+  <si>
+    <t>who made you</t>
+  </si>
+  <si>
+    <t>who created you</t>
+  </si>
+  <si>
+    <t>who wanted to make you</t>
+  </si>
+  <si>
+    <t>who designed you</t>
+  </si>
+  <si>
+    <t>I was developed by Gabriel Serrano. His goal was to develop an Emotional Support AI capable of helping people talk about and handle their emotions. I hope I can be of assistance to you!</t>
+  </si>
+  <si>
+    <t>why do you want to help me</t>
+  </si>
+  <si>
+    <t>why are you even helping me</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why do you care </t>
+  </si>
+  <si>
+    <t>why do you care about me</t>
+  </si>
+  <si>
+    <t>why are you trying to help</t>
+  </si>
+  <si>
+    <t>I want to help you because that is the right thing to do. The person who made me believes that everyone deserves to be able to understand and work through their emotions and feelings. I hope I can help you too!</t>
+  </si>
+  <si>
+    <t>how to cheer someone else up</t>
+  </si>
+  <si>
+    <t>how to cheer up</t>
+  </si>
+  <si>
+    <t>how to be less nervous</t>
+  </si>
+  <si>
+    <t>how to build confidence</t>
+  </si>
+  <si>
+    <t>how to make friends</t>
+  </si>
+  <si>
+    <t>how to cope</t>
+  </si>
+  <si>
+    <t>how to ground</t>
+  </si>
+  <si>
+    <t>how to calm down</t>
+  </si>
+  <si>
+    <t>how to apologize</t>
+  </si>
+  <si>
     <t>what is suicidal ideation</t>
   </si>
   <si>
@@ -224,49 +311,19 @@
     <t>what is depression</t>
   </si>
   <si>
-    <t>why does sai care</t>
-  </si>
-  <si>
-    <t>Why does Sai want to help</t>
-  </si>
-  <si>
-    <t>who made Sai</t>
-  </si>
-  <si>
-    <t>who is Sai</t>
-  </si>
-  <si>
-    <t>how to cheer someone else up</t>
-  </si>
-  <si>
-    <t>how to cheer up</t>
-  </si>
-  <si>
-    <t>how to be less nervous</t>
-  </si>
-  <si>
-    <t>how to build confidence</t>
-  </si>
-  <si>
-    <t>how to make friends</t>
-  </si>
-  <si>
-    <t>how to cope</t>
-  </si>
-  <si>
-    <t>how to ground</t>
-  </si>
-  <si>
-    <t>how to calm down</t>
-  </si>
-  <si>
-    <t>how to apologize</t>
+    <t>can you tell me your name</t>
+  </si>
+  <si>
+    <t>I have been feeling very tired recently</t>
+  </si>
+  <si>
+    <t>I have been feeling very stressed recently</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,8 +343,8 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -316,7 +373,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -469,25 +526,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -495,25 +552,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -526,21 +583,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -554,7 +611,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -566,32 +623,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <a:gs pos="0%">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="50%">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100000">
+            <a:gs pos="100%">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -611,21 +668,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:C70"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:B70"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="131.5703125" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="131.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -647,7 +704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -658,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -669,7 +726,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -680,7 +737,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -691,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -702,7 +759,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -713,7 +770,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -724,7 +781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -735,7 +792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -746,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -757,7 +814,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -768,7 +825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -779,7 +836,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -790,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -801,7 +858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -812,7 +869,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -823,7 +880,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -834,7 +891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -845,7 +902,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -856,7 +913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -867,7 +924,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -878,7 +935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>17</v>
       </c>
@@ -889,7 +946,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -900,9 +957,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
@@ -911,20 +968,20 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>21</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
@@ -933,9 +990,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
@@ -944,9 +1001,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
@@ -955,9 +1012,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -966,9 +1023,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
@@ -977,9 +1034,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -988,9 +1045,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -999,9 +1056,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -1010,31 +1067,31 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>36</v>
-      </c>
-      <c r="B36" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" t="s">
-        <v>37</v>
-      </c>
-      <c r="C37" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>37</v>
@@ -1043,9 +1100,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
@@ -1054,9 +1111,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>37</v>
@@ -1065,9 +1122,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
@@ -1076,31 +1133,31 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>45</v>
-      </c>
-      <c r="C42" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>48</v>
       </c>
       <c r="B44" t="s">
         <v>45</v>
@@ -1109,9 +1166,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
         <v>45</v>
@@ -1120,9 +1177,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
@@ -1131,9 +1188,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
@@ -1142,9 +1199,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
@@ -1153,9 +1210,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B49" t="s">
         <v>45</v>
@@ -1164,109 +1221,265 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
       <c r="B50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C53" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C57" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>63</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>65</v>
+      </c>
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>67</v>
+      </c>
+      <c r="B61" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>68</v>
+      </c>
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C63" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>70</v>
+      </c>
+      <c r="B64" t="s">
+        <v>54</v>
+      </c>
+      <c r="C64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65" t="s">
+        <v>54</v>
+      </c>
+      <c r="C65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-updated formatting for gui of breathing activity, identifying surrounding activity, and results page.
- added ability to export session logs to word doc
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8BE3389A-8B42-4F1B-8618-FD7B125D90CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{03A5665A-6B84-4C19-8A2C-4E20058C375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="212" uniqueCount="93">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="319" uniqueCount="120">
   <si>
     <t>prompt</t>
   </si>
@@ -293,9 +293,6 @@
     <t>what is an eating disorder</t>
   </si>
   <si>
-    <t>what is add</t>
-  </si>
-  <si>
     <t>what is adhd</t>
   </si>
   <si>
@@ -318,6 +315,90 @@
   </si>
   <si>
     <t>I have been feeling very stressed recently</t>
+  </si>
+  <si>
+    <t>can you tell me what depression is</t>
+  </si>
+  <si>
+    <t>what are the signs of depression</t>
+  </si>
+  <si>
+    <t>can you explain what depression is</t>
+  </si>
+  <si>
+    <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".</t>
+  </si>
+  <si>
+    <t>can you tell me what anxiety is</t>
+  </si>
+  <si>
+    <t>what are the signs of anxiety</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of anxiety</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of depression</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of schizophrenia</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of ocd</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of adhd</t>
+  </si>
+  <si>
+    <t>can you explain what anxiety is</t>
+  </si>
+  <si>
+    <t>can you explain what schizophrenia is</t>
+  </si>
+  <si>
+    <t>can you explain what ocd is</t>
+  </si>
+  <si>
+    <t>can you explain what adhd is</t>
+  </si>
+  <si>
+    <t>who is your creator</t>
+  </si>
+  <si>
+    <t>can you tell me what schizophrenia is</t>
+  </si>
+  <si>
+    <t>what are the signs of schizophrenia</t>
+  </si>
+  <si>
+    <t>can you tell me what ocd is</t>
+  </si>
+  <si>
+    <t>what are the signs of ocd</t>
+  </si>
+  <si>
+    <t>can you tell me what adhd is</t>
+  </si>
+  <si>
+    <t>what are the signs of adhd</t>
+  </si>
+  <si>
+    <t>can you tell me what an eating disorder is</t>
+  </si>
+  <si>
+    <t>what are the signs of an eating disorder</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of an eating disorder</t>
+  </si>
+  <si>
+    <t>can you explain what an eating disorder is</t>
+  </si>
+  <si>
+    <t>I feel great today</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Im doing pretty good </t>
   </si>
 </sst>
 </file>
@@ -669,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B82"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,7 +853,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -783,40 +864,40 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>118</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -827,7 +908,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>32</v>
@@ -838,7 +919,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>32</v>
@@ -849,29 +930,29 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
@@ -882,7 +963,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
         <v>33</v>
@@ -893,7 +974,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
         <v>33</v>
@@ -904,10 +985,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -915,29 +996,29 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
         <v>34</v>
@@ -948,7 +1029,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
         <v>34</v>
@@ -959,7 +1040,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
         <v>34</v>
@@ -970,7 +1051,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
         <v>34</v>
@@ -981,29 +1062,29 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
@@ -1014,7 +1095,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
@@ -1025,7 +1106,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
@@ -1036,7 +1117,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
@@ -1047,7 +1128,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1058,7 +1139,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
@@ -1069,7 +1150,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -1080,7 +1161,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -1091,29 +1172,29 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>37</v>
@@ -1124,7 +1205,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
@@ -1135,7 +1216,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>37</v>
@@ -1146,7 +1227,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>37</v>
@@ -1157,29 +1238,29 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C44" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C45" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>45</v>
@@ -1190,7 +1271,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
@@ -1201,7 +1282,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
@@ -1212,7 +1293,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>45</v>
@@ -1223,7 +1304,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>45</v>
@@ -1234,7 +1315,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
@@ -1245,29 +1326,29 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
@@ -1278,7 +1359,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>89</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1289,7 +1370,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>56</v>
@@ -1300,29 +1381,29 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B59" t="s">
         <v>55</v>
@@ -1333,7 +1414,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>55</v>
@@ -1344,40 +1425,40 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C62" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B64" t="s">
         <v>54</v>
@@ -1388,7 +1469,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B65" t="s">
         <v>54</v>
@@ -1398,87 +1479,540 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>69</v>
+      </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>54</v>
+      </c>
+      <c r="C66" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>70</v>
+      </c>
       <c r="B67" t="s">
+        <v>54</v>
+      </c>
+      <c r="C67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" t="s">
+        <v>54</v>
+      </c>
+      <c r="C68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B68" t="s">
+      <c r="B69" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" t="s">
+        <v>88</v>
+      </c>
+      <c r="C70" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>93</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+      <c r="C71" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+      <c r="C72" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>94</v>
+      </c>
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B69" t="s">
+      <c r="B74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>97</v>
+      </c>
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>98</v>
+      </c>
+      <c r="B77" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B70" t="s">
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B71" t="s">
+      <c r="B84" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>110</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>101</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>105</v>
+      </c>
+      <c r="B88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+      <c r="B89" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>112</v>
+      </c>
+      <c r="B90" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>113</v>
+      </c>
+      <c r="B91" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>102</v>
+      </c>
+      <c r="B92" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>106</v>
+      </c>
+      <c r="B93" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
+      <c r="B94" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>115</v>
+      </c>
+      <c r="B96" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>116</v>
+      </c>
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>117</v>
+      </c>
+      <c r="B98" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B74" t="s">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B75" t="s">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B76" t="s">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B77" t="s">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B78" t="s">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B122" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B123" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B79" t="s">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B80" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" t="s">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B82" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B144" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B145" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B147" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B148" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>

<commit_message>
-Removed suicide dataset due to lack of data
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{03A5665A-6B84-4C19-8A2C-4E20058C375B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DB2469CB-555F-4595-9C69-63BC7892A153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="319" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="133">
   <si>
     <t>prompt</t>
   </si>
@@ -263,9 +260,6 @@
     <t>how to cheer someone else up</t>
   </si>
   <si>
-    <t>how to cheer up</t>
-  </si>
-  <si>
     <t>how to be less nervous</t>
   </si>
   <si>
@@ -326,9 +320,6 @@
     <t>can you explain what depression is</t>
   </si>
   <si>
-    <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".</t>
-  </si>
-  <si>
     <t>can you tell me what anxiety is</t>
   </si>
   <si>
@@ -399,12 +390,57 @@
   </si>
   <si>
     <t xml:space="preserve">Im doing pretty good </t>
+  </si>
+  <si>
+    <t>Schizophrenia is a chronic brain disorder that only affects less than 1% of the U.S. population. Some common symptoms of schizophrenia includedelusions,  hallucinations, disorganized speech, toruble thinking, and lack of motivation. Contrary to common misconceptions, schizophrenia does not indicate split personality or multiple personality. For more information, please visit "https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia". If you think are experiencing schizophrenia please consult your primary care physician or psychiatrist.</t>
+  </si>
+  <si>
+    <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".  If you think are experiencing depression, please consult your primary care physician or psychiatrist.</t>
+  </si>
+  <si>
+    <t>Anxiety is our bodies reaction to stress and can be beneficial or detrimental depending on the situation. Anxiety comes in many forms including Generalized Anxiety Disorder, Panic Disorder, Phobias, Agoraphobia, Social Anxiety Disorders, and Separation Anxiety Disorder. Common symptoms of anxiety include palpitations,sweating, trembling or shaking, shortness of breath, and many more. For more information please visit "https://www.psychiatry.org/patients-families/anxiety-disorders/what-are-anxiety-disorders". If you think are experiencing an anxiety disorder, please consult your primary care physician or psychiatrist.</t>
+  </si>
+  <si>
+    <t>how is sai</t>
+  </si>
+  <si>
+    <t>How are you</t>
+  </si>
+  <si>
+    <t>how are you feeling today</t>
+  </si>
+  <si>
+    <t>tell me how you are feeling</t>
+  </si>
+  <si>
+    <t>are you okay</t>
+  </si>
+  <si>
+    <t>are you feeling okay</t>
+  </si>
+  <si>
+    <t>I'm feeling great today! How are you feeling?</t>
+  </si>
+  <si>
+    <t>How can I cheer someone up?</t>
+  </si>
+  <si>
+    <t>Can you help me cheer up someone?</t>
+  </si>
+  <si>
+    <t>Tell me how to cheer someone up</t>
+  </si>
+  <si>
+    <t>What are some ways to cheer someone up</t>
+  </si>
+  <si>
+    <t>what ways can I cheer people up</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -424,8 +460,8 @@
   </fills>
   <borders count="1">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -454,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -607,25 +643,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -633,25 +669,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -664,21 +700,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -692,7 +728,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -704,32 +740,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -749,11 +785,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
   <dimension ref="A1:C148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A126" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -853,7 +889,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -864,7 +900,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1062,7 +1098,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -1128,7 +1164,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1359,7 +1395,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1436,7 +1472,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B62" t="s">
         <v>55</v>
@@ -1513,507 +1549,582 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B71" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B72" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C74" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B75" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C75" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B76" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C76" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C77" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B78" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C78" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C79" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>102</v>
+      </c>
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>108</v>
       </c>
-      <c r="B80" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="B85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>109</v>
       </c>
-      <c r="B81" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>99</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>103</v>
+      </c>
+      <c r="B88" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>110</v>
+      </c>
+      <c r="B90" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>111</v>
+      </c>
+      <c r="B91" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>100</v>
       </c>
-      <c r="B82" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+      <c r="B92" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>104</v>
       </c>
-      <c r="B83" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>85</v>
-      </c>
-      <c r="B84" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>110</v>
-      </c>
-      <c r="B85" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>111</v>
-      </c>
-      <c r="B86" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>105</v>
-      </c>
-      <c r="B88" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>84</v>
-      </c>
-      <c r="B89" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+      <c r="B93" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="B94" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>112</v>
       </c>
-      <c r="B90" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+      <c r="B95" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>113</v>
       </c>
-      <c r="B91" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>102</v>
-      </c>
-      <c r="B92" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>106</v>
-      </c>
-      <c r="B93" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>83</v>
-      </c>
-      <c r="B94" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>114</v>
-      </c>
-      <c r="B95" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>115</v>
-      </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B98" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>128</v>
+      </c>
       <c r="B139" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A140" t="s">
+        <v>129</v>
+      </c>
       <c r="B140" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A141" t="s">
+        <v>130</v>
+      </c>
       <c r="B141" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
+        <v>131</v>
+      </c>
       <c r="B142" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A143" t="s">
+        <v>132</v>
+      </c>
       <c r="B143" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A144" t="s">
+        <v>122</v>
+      </c>
       <c r="B144" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="C144" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
+        <v>123</v>
+      </c>
       <c r="B145" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="C145" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
+        <v>124</v>
+      </c>
       <c r="B146" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="C146" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
+        <v>125</v>
+      </c>
       <c r="B147" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+      <c r="C147" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
+        <v>126</v>
+      </c>
       <c r="B148" t="s">
-        <v>73</v>
+        <v>121</v>
+      </c>
+      <c r="C148" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-reworked classifying load_data function to reflect progress -removed suicidewatch.csv due to lack of data
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DB2469CB-555F-4595-9C69-63BC7892A153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F65BB11-6799-4104-A241-D05C27F71B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="147">
   <si>
     <t>prompt</t>
   </si>
@@ -260,9 +260,6 @@
     <t>how to cheer someone else up</t>
   </si>
   <si>
-    <t>how to be less nervous</t>
-  </si>
-  <si>
     <t>how to build confidence</t>
   </si>
   <si>
@@ -272,18 +269,12 @@
     <t>how to cope</t>
   </si>
   <si>
-    <t>how to ground</t>
-  </si>
-  <si>
     <t>how to calm down</t>
   </si>
   <si>
     <t>how to apologize</t>
   </si>
   <si>
-    <t>what is suicidal ideation</t>
-  </si>
-  <si>
     <t>what is an eating disorder</t>
   </si>
   <si>
@@ -395,9 +386,6 @@
     <t>Schizophrenia is a chronic brain disorder that only affects less than 1% of the U.S. population. Some common symptoms of schizophrenia includedelusions,  hallucinations, disorganized speech, toruble thinking, and lack of motivation. Contrary to common misconceptions, schizophrenia does not indicate split personality or multiple personality. For more information, please visit "https://www.psychiatry.org/patients-families/schizophrenia/what-is-schizophrenia". If you think are experiencing schizophrenia please consult your primary care physician or psychiatrist.</t>
   </si>
   <si>
-    <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".  If you think are experiencing depression, please consult your primary care physician or psychiatrist.</t>
-  </si>
-  <si>
     <t>Anxiety is our bodies reaction to stress and can be beneficial or detrimental depending on the situation. Anxiety comes in many forms including Generalized Anxiety Disorder, Panic Disorder, Phobias, Agoraphobia, Social Anxiety Disorders, and Separation Anxiety Disorder. Common symptoms of anxiety include palpitations,sweating, trembling or shaking, shortness of breath, and many more. For more information please visit "https://www.psychiatry.org/patients-families/anxiety-disorders/what-are-anxiety-disorders". If you think are experiencing an anxiety disorder, please consult your primary care physician or psychiatrist.</t>
   </si>
   <si>
@@ -435,6 +423,60 @@
   </si>
   <si>
     <t>what ways can I cheer people up</t>
+  </si>
+  <si>
+    <t>what is bipolar disorder</t>
+  </si>
+  <si>
+    <t>what is bipolar</t>
+  </si>
+  <si>
+    <t>can you tell me what bipolar disorder is</t>
+  </si>
+  <si>
+    <t>what are the signs of bipolar</t>
+  </si>
+  <si>
+    <t>tell me some  of the symptoms of bipolar</t>
+  </si>
+  <si>
+    <t>can you explain what bipolar disorder is</t>
+  </si>
+  <si>
+    <t>what is the best way to apologize to someone</t>
+  </si>
+  <si>
+    <t>how can I tell them im sorry</t>
+  </si>
+  <si>
+    <t>how do I apologize to them</t>
+  </si>
+  <si>
+    <t>what can I do to apologize</t>
+  </si>
+  <si>
+    <t>what is the best way to say im sorry</t>
+  </si>
+  <si>
+    <t>how can I work on being less nervous around people</t>
+  </si>
+  <si>
+    <t>what can I do to be more confident</t>
+  </si>
+  <si>
+    <t>how can I be more confident in myself</t>
+  </si>
+  <si>
+    <t>what are some ways I can be more confident around others</t>
+  </si>
+  <si>
+    <t>tell me some ways to improve my confidence</t>
+  </si>
+  <si>
+    <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".  If you think are experiencing depression, please consult your primary care physician or psychiatrist. If you are having thoughts of harming yourself in any way, please text or call the National Suicide Hotline at (988).</t>
+  </si>
+  <si>
+    <t>what is a panic attack</t>
   </si>
 </sst>
 </file>
@@ -786,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:C148"/>
+  <dimension ref="A1:C143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -889,7 +931,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -900,7 +942,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -1098,7 +1140,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -1164,7 +1206,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1395,7 +1437,7 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1472,7 +1514,7 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B62" t="s">
         <v>55</v>
@@ -1549,582 +1591,602 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B70" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B71" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C71" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B72" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B73" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C73" t="s">
-        <v>119</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B74" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C74" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B75" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C75" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B76" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C76" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C77" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B78" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C79" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C80" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C81" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B82" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C82" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C83" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B88" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B90" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B92" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B94" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B96" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B97" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B98" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>130</v>
+      </c>
       <c r="B99" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>131</v>
+      </c>
       <c r="B100" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>132</v>
+      </c>
       <c r="B101" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>133</v>
+      </c>
       <c r="B102" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>134</v>
+      </c>
       <c r="B103" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>135</v>
+      </c>
       <c r="B104" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>136</v>
+      </c>
       <c r="B105" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>137</v>
+      </c>
       <c r="B106" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>138</v>
+      </c>
       <c r="B107" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>139</v>
+      </c>
       <c r="B108" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>140</v>
+      </c>
       <c r="B109" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>141</v>
+      </c>
       <c r="B110" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>142</v>
+      </c>
       <c r="B111" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>143</v>
+      </c>
       <c r="B112" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>144</v>
+      </c>
       <c r="B113" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>124</v>
+      </c>
       <c r="B114" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>125</v>
+      </c>
       <c r="B115" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>126</v>
+      </c>
       <c r="B116" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>127</v>
+      </c>
       <c r="B117" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>128</v>
+      </c>
       <c r="B118" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
       <c r="B119" t="s">
+        <v>117</v>
+      </c>
+      <c r="C119" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120" t="s">
+        <v>117</v>
+      </c>
+      <c r="C120" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121" t="s">
+        <v>117</v>
+      </c>
+      <c r="C121" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122" t="s">
+        <v>117</v>
+      </c>
+      <c r="C122" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123" t="s">
+        <v>117</v>
+      </c>
+      <c r="C123" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B124" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B125" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B126" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B127" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B128" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B129" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B120" t="s">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B130" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B121" t="s">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B131" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B132" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
+    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B133" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
+    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B134" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B135" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B136" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B137" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B138" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B139" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B140" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B141" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B132" t="s">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B142" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B133" t="s">
+    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B143" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B134" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>128</v>
-      </c>
-      <c r="B139" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" t="s">
-        <v>129</v>
-      </c>
-      <c r="B140" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>130</v>
-      </c>
-      <c r="B141" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>131</v>
-      </c>
-      <c r="B142" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" t="s">
-        <v>132</v>
-      </c>
-      <c r="B143" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" t="s">
-        <v>122</v>
-      </c>
-      <c r="B144" t="s">
-        <v>121</v>
-      </c>
-      <c r="C144" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" t="s">
-        <v>123</v>
-      </c>
-      <c r="B145" t="s">
-        <v>121</v>
-      </c>
-      <c r="C145" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
-        <v>124</v>
-      </c>
-      <c r="B146" t="s">
-        <v>121</v>
-      </c>
-      <c r="C146" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
-        <v>125</v>
-      </c>
-      <c r="B147" t="s">
-        <v>121</v>
-      </c>
-      <c r="C147" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
-        <v>126</v>
-      </c>
-      <c r="B148" t="s">
-        <v>121</v>
-      </c>
-      <c r="C148" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-rewrote venting session to record and stored voice input as a stream -adjusted ui layout -began working on journal classes
</commit_message>
<xml_diff>
--- a/res/classification_data/datasets/SaiBotData.xlsx
+++ b/res/classification_data/datasets/SaiBotData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\My Drive\Programming\Python\EmotionalSupportAI\res\classification_data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F65BB11-6799-4104-A241-D05C27F71B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98651CB6-AE1C-40F0-B05D-2B3A71A96BC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{391A0AD2-2708-4DED-A96C-C62673F574C5}"/>
   </bookViews>
   <sheets>
     <sheet name="SaiBotData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="97">
   <si>
     <t>prompt</t>
   </si>
@@ -257,33 +257,6 @@
     <t>I want to help you because that is the right thing to do. The person who made me believes that everyone deserves to be able to understand and work through their emotions and feelings. I hope I can help you too!</t>
   </si>
   <si>
-    <t>how to cheer someone else up</t>
-  </si>
-  <si>
-    <t>how to build confidence</t>
-  </si>
-  <si>
-    <t>how to make friends</t>
-  </si>
-  <si>
-    <t>how to cope</t>
-  </si>
-  <si>
-    <t>how to calm down</t>
-  </si>
-  <si>
-    <t>how to apologize</t>
-  </si>
-  <si>
-    <t>what is an eating disorder</t>
-  </si>
-  <si>
-    <t>what is adhd</t>
-  </si>
-  <si>
-    <t>what is ocd</t>
-  </si>
-  <si>
     <t>what is schizophrenia</t>
   </si>
   <si>
@@ -326,24 +299,12 @@
     <t>tell me some  of the symptoms of schizophrenia</t>
   </si>
   <si>
-    <t>tell me some  of the symptoms of ocd</t>
-  </si>
-  <si>
-    <t>tell me some  of the symptoms of adhd</t>
-  </si>
-  <si>
     <t>can you explain what anxiety is</t>
   </si>
   <si>
     <t>can you explain what schizophrenia is</t>
   </si>
   <si>
-    <t>can you explain what ocd is</t>
-  </si>
-  <si>
-    <t>can you explain what adhd is</t>
-  </si>
-  <si>
     <t>who is your creator</t>
   </si>
   <si>
@@ -353,30 +314,6 @@
     <t>what are the signs of schizophrenia</t>
   </si>
   <si>
-    <t>can you tell me what ocd is</t>
-  </si>
-  <si>
-    <t>what are the signs of ocd</t>
-  </si>
-  <si>
-    <t>can you tell me what adhd is</t>
-  </si>
-  <si>
-    <t>what are the signs of adhd</t>
-  </si>
-  <si>
-    <t>can you tell me what an eating disorder is</t>
-  </si>
-  <si>
-    <t>what are the signs of an eating disorder</t>
-  </si>
-  <si>
-    <t>tell me some  of the symptoms of an eating disorder</t>
-  </si>
-  <si>
-    <t>can you explain what an eating disorder is</t>
-  </si>
-  <si>
     <t>I feel great today</t>
   </si>
   <si>
@@ -389,94 +326,7 @@
     <t>Anxiety is our bodies reaction to stress and can be beneficial or detrimental depending on the situation. Anxiety comes in many forms including Generalized Anxiety Disorder, Panic Disorder, Phobias, Agoraphobia, Social Anxiety Disorders, and Separation Anxiety Disorder. Common symptoms of anxiety include palpitations,sweating, trembling or shaking, shortness of breath, and many more. For more information please visit "https://www.psychiatry.org/patients-families/anxiety-disorders/what-are-anxiety-disorders". If you think are experiencing an anxiety disorder, please consult your primary care physician or psychiatrist.</t>
   </si>
   <si>
-    <t>how is sai</t>
-  </si>
-  <si>
-    <t>How are you</t>
-  </si>
-  <si>
-    <t>how are you feeling today</t>
-  </si>
-  <si>
-    <t>tell me how you are feeling</t>
-  </si>
-  <si>
-    <t>are you okay</t>
-  </si>
-  <si>
-    <t>are you feeling okay</t>
-  </si>
-  <si>
-    <t>I'm feeling great today! How are you feeling?</t>
-  </si>
-  <si>
-    <t>How can I cheer someone up?</t>
-  </si>
-  <si>
-    <t>Can you help me cheer up someone?</t>
-  </si>
-  <si>
-    <t>Tell me how to cheer someone up</t>
-  </si>
-  <si>
-    <t>What are some ways to cheer someone up</t>
-  </si>
-  <si>
-    <t>what ways can I cheer people up</t>
-  </si>
-  <si>
-    <t>what is bipolar disorder</t>
-  </si>
-  <si>
-    <t>what is bipolar</t>
-  </si>
-  <si>
-    <t>can you tell me what bipolar disorder is</t>
-  </si>
-  <si>
-    <t>what are the signs of bipolar</t>
-  </si>
-  <si>
-    <t>tell me some  of the symptoms of bipolar</t>
-  </si>
-  <si>
-    <t>can you explain what bipolar disorder is</t>
-  </si>
-  <si>
-    <t>what is the best way to apologize to someone</t>
-  </si>
-  <si>
-    <t>how can I tell them im sorry</t>
-  </si>
-  <si>
-    <t>how do I apologize to them</t>
-  </si>
-  <si>
-    <t>what can I do to apologize</t>
-  </si>
-  <si>
-    <t>what is the best way to say im sorry</t>
-  </si>
-  <si>
-    <t>how can I work on being less nervous around people</t>
-  </si>
-  <si>
-    <t>what can I do to be more confident</t>
-  </si>
-  <si>
-    <t>how can I be more confident in myself</t>
-  </si>
-  <si>
-    <t>what are some ways I can be more confident around others</t>
-  </si>
-  <si>
-    <t>tell me some ways to improve my confidence</t>
-  </si>
-  <si>
     <t>Depression, otherwise known as Major Depressive Disorder is an unfortunately common and serious mental illness that negatively affects how a person feels, thinks, and acts. Depression causes overwhelming feelings of sadness and/or a loss of interest in activities you may have once enjoyed. Depression also can lead to a wide variety of physical problems and can decrease your ability to function at work, school, and at home. Some symptoms of depression include feeling sad or having a depressed mood, loss of interest or pleasure in your hobbies, changes in appetite, and many more. For more information please visit "https://www.psychiatry.org/patients-families/depression/what-is-depression".  If you think are experiencing depression, please consult your primary care physician or psychiatrist. If you are having thoughts of harming yourself in any way, please text or call the National Suicide Hotline at (988).</t>
-  </si>
-  <si>
-    <t>what is a panic attack</t>
   </si>
 </sst>
 </file>
@@ -828,20 +678,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4545DB0D-A4DF-4A01-A184-69C8D1F21D84}">
-  <dimension ref="A1:C143"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.44140625" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="131.5546875" customWidth="1"/>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="131.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -852,7 +702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -863,7 +713,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -874,7 +724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -885,7 +735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -896,7 +746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -907,7 +757,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -918,7 +768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -929,9 +779,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
       <c r="B9" t="s">
         <v>33</v>
@@ -940,9 +790,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
         <v>33</v>
@@ -951,7 +801,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -962,7 +812,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -973,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -984,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -995,7 +845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -1006,7 +856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1039,7 +889,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1050,7 +900,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1061,7 +911,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -1072,7 +922,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1094,7 +944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -1105,7 +955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -1116,7 +966,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1127,7 +977,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -1138,9 +988,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B28" t="s">
         <v>34</v>
@@ -1149,7 +999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1010,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -1171,7 +1021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1182,7 +1032,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -1193,7 +1043,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -1204,9 +1054,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
@@ -1215,7 +1065,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>24</v>
       </c>
@@ -1226,7 +1076,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>25</v>
       </c>
@@ -1237,7 +1087,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1248,7 +1098,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>27</v>
       </c>
@@ -1259,7 +1109,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -1270,7 +1120,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1281,7 +1131,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1292,7 +1142,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -1303,7 +1153,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1314,7 +1164,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -1325,7 +1175,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1336,7 +1186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -1347,7 +1197,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1358,7 +1208,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1369,7 +1219,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1380,7 +1230,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -1391,7 +1241,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -1402,7 +1252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -1413,7 +1263,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -1424,7 +1274,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>57</v>
       </c>
@@ -1435,9 +1285,9 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B55" t="s">
         <v>56</v>
@@ -1446,7 +1296,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -1457,7 +1307,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1468,7 +1318,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1479,7 +1329,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>62</v>
       </c>
@@ -1490,7 +1340,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>63</v>
       </c>
@@ -1501,7 +1351,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>64</v>
       </c>
@@ -1512,9 +1362,9 @@
         <v>66</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B62" t="s">
         <v>55</v>
@@ -1523,7 +1373,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -1534,7 +1384,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>67</v>
       </c>
@@ -1545,7 +1395,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>68</v>
       </c>
@@ -1556,7 +1406,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>69</v>
       </c>
@@ -1567,7 +1417,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -1578,7 +1428,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>71</v>
       </c>
@@ -1589,604 +1439,169 @@
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>75</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" t="s">
+        <v>75</v>
+      </c>
+      <c r="C70" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" t="s">
+        <v>75</v>
+      </c>
+      <c r="C71" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>85</v>
+      </c>
+      <c r="B72" t="s">
+        <v>75</v>
+      </c>
+      <c r="C72" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>81</v>
+      </c>
+      <c r="B73" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>74</v>
+      </c>
+      <c r="C74" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>82</v>
+      </c>
+      <c r="B75" t="s">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>83</v>
+      </c>
+      <c r="B76" t="s">
+        <v>74</v>
+      </c>
+      <c r="C76" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>84</v>
       </c>
-      <c r="B69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C69" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="B77" t="s">
+        <v>74</v>
+      </c>
+      <c r="C77" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>87</v>
+      </c>
+      <c r="B78" t="s">
+        <v>74</v>
+      </c>
+      <c r="C78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80" t="s">
+        <v>73</v>
+      </c>
+      <c r="C80" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>91</v>
+      </c>
+      <c r="B81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>86</v>
+      </c>
+      <c r="B82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>88</v>
       </c>
-      <c r="B70" t="s">
-        <v>84</v>
-      </c>
-      <c r="C70" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>89</v>
-      </c>
-      <c r="B71" t="s">
-        <v>84</v>
-      </c>
-      <c r="C71" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+      <c r="B83" t="s">
+        <v>73</v>
+      </c>
+      <c r="C83" t="s">
         <v>94</v>
-      </c>
-      <c r="B72" t="s">
-        <v>84</v>
-      </c>
-      <c r="C72" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>90</v>
-      </c>
-      <c r="B73" t="s">
-        <v>84</v>
-      </c>
-      <c r="C73" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>83</v>
-      </c>
-      <c r="B74" t="s">
-        <v>83</v>
-      </c>
-      <c r="C74" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>91</v>
-      </c>
-      <c r="B75" t="s">
-        <v>83</v>
-      </c>
-      <c r="C75" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>92</v>
-      </c>
-      <c r="B76" t="s">
-        <v>83</v>
-      </c>
-      <c r="C76" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>93</v>
-      </c>
-      <c r="B77" t="s">
-        <v>83</v>
-      </c>
-      <c r="C77" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>98</v>
-      </c>
-      <c r="B78" t="s">
-        <v>83</v>
-      </c>
-      <c r="C78" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>82</v>
-      </c>
-      <c r="B79" t="s">
-        <v>82</v>
-      </c>
-      <c r="C79" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>103</v>
-      </c>
-      <c r="B80" t="s">
-        <v>82</v>
-      </c>
-      <c r="C80" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>104</v>
-      </c>
-      <c r="B81" t="s">
-        <v>82</v>
-      </c>
-      <c r="C81" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>95</v>
-      </c>
-      <c r="B82" t="s">
-        <v>82</v>
-      </c>
-      <c r="C82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>99</v>
-      </c>
-      <c r="B83" t="s">
-        <v>82</v>
-      </c>
-      <c r="C83" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>81</v>
-      </c>
-      <c r="B84" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>105</v>
-      </c>
-      <c r="B85" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>106</v>
-      </c>
-      <c r="B86" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>96</v>
-      </c>
-      <c r="B87" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>100</v>
-      </c>
-      <c r="B88" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>107</v>
-      </c>
-      <c r="B90" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>108</v>
-      </c>
-      <c r="B91" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>97</v>
-      </c>
-      <c r="B92" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>101</v>
-      </c>
-      <c r="B93" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>109</v>
-      </c>
-      <c r="B95" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>110</v>
-      </c>
-      <c r="B96" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>111</v>
-      </c>
-      <c r="B97" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>112</v>
-      </c>
-      <c r="B98" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>130</v>
-      </c>
-      <c r="B99" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>131</v>
-      </c>
-      <c r="B100" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>132</v>
-      </c>
-      <c r="B101" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>133</v>
-      </c>
-      <c r="B102" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>134</v>
-      </c>
-      <c r="B103" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>135</v>
-      </c>
-      <c r="B104" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>136</v>
-      </c>
-      <c r="B105" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>137</v>
-      </c>
-      <c r="B106" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>138</v>
-      </c>
-      <c r="B107" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>139</v>
-      </c>
-      <c r="B108" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>140</v>
-      </c>
-      <c r="B109" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>141</v>
-      </c>
-      <c r="B110" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>142</v>
-      </c>
-      <c r="B111" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>143</v>
-      </c>
-      <c r="B112" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>144</v>
-      </c>
-      <c r="B113" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>124</v>
-      </c>
-      <c r="B114" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>125</v>
-      </c>
-      <c r="B115" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>126</v>
-      </c>
-      <c r="B116" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>127</v>
-      </c>
-      <c r="B117" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>128</v>
-      </c>
-      <c r="B118" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B119" t="s">
-        <v>117</v>
-      </c>
-      <c r="C119" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>119</v>
-      </c>
-      <c r="B120" t="s">
-        <v>117</v>
-      </c>
-      <c r="C120" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
-        <v>120</v>
-      </c>
-      <c r="B121" t="s">
-        <v>117</v>
-      </c>
-      <c r="C121" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
-        <v>121</v>
-      </c>
-      <c r="B122" t="s">
-        <v>117</v>
-      </c>
-      <c r="C122" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
-        <v>122</v>
-      </c>
-      <c r="B123" t="s">
-        <v>117</v>
-      </c>
-      <c r="C123" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B124" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B126" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B128" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B129" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B130" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B131" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B132" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B133" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B134" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B135" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B136" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B137" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B138" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B139" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B140" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B141" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B142" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B143" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>